<commit_message>
Updated content issues for recuresive scenarios Added spinner to send feeback screen Updated pause menu to make send feedback look like a button
</commit_message>
<xml_diff>
--- a/Assets/Resources/RFScenarios/Belfast/AllBelfastScenarios.xlsx
+++ b/Assets/Resources/RFScenarios/Belfast/AllBelfastScenarios.xlsx
@@ -865,49 +865,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -1211,8 +1169,8 @@
   <dimension ref="A1:Z959"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3630,7 +3588,7 @@
         <v>4</v>
       </c>
       <c r="G40" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H40" s="8">
         <v>1</v>
@@ -30640,12 +30598,12 @@
     <mergeCell ref="E1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:G2 E10:G959">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Q1048576">
-    <cfRule type="containsBlanks" dxfId="6" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Edit incident retrieval to be more stable with less incidents, causing while locks in belfast at end of turn update misssing resolution string for belfast
</commit_message>
<xml_diff>
--- a/Assets/Resources/RFScenarios/Belfast/AllBelfastScenarios.xlsx
+++ b/Assets/Resources/RFScenarios/Belfast/AllBelfastScenarios.xlsx
@@ -1169,8 +1169,8 @@
   <dimension ref="A1:Z959"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
+      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4459,10 +4459,10 @@
         <v>-1</v>
       </c>
       <c r="H54" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I54" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J54" s="2">
         <v>3</v>

</xml_diff>

<commit_message>
All content updated to use new format as with authoring tool Translations for scenarios now saved as its own scenario data to make it maths authoring tool structure
</commit_message>
<xml_diff>
--- a/Assets/Resources/RFScenarios/Belfast/AllBelfastScenarios.xlsx
+++ b/Assets/Resources/RFScenarios/Belfast/AllBelfastScenarios.xlsx
@@ -1170,7 +1170,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H77" sqref="H77"/>
+      <selection pane="bottomLeft" activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3706,13 +3706,13 @@
         <v>133</v>
       </c>
       <c r="E42" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F42" s="8">
         <v>-1</v>
       </c>
       <c r="G42" s="8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H42" s="8">
         <v>0</v>

</xml_diff>